<commit_message>
policy verification and add payment page verification
</commit_message>
<xml_diff>
--- a/src/test/resources/Life Insurance.xlsx
+++ b/src/test/resources/Life Insurance.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="13" documentId="6_{F7E9FF1E-DF67-4470-BFF9-B8A28275E406}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E2698548-4EB3-45A4-B642-11C5098691AB}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AddClient" sheetId="1" r:id="rId1"/>
     <sheet name="AddNominee" sheetId="2" r:id="rId2"/>
     <sheet name="Payment " sheetId="6" r:id="rId3"/>
     <sheet name="SearchPage" sheetId="3" r:id="rId4"/>
-    <sheet name="Policy" sheetId="4" r:id="rId5"/>
+    <sheet name="policy" sheetId="4" r:id="rId5"/>
     <sheet name="Agents" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>Client Password</t>
   </si>
@@ -208,12 +207,36 @@
   </si>
   <si>
     <t>Phone num</t>
+  </si>
+  <si>
+    <t>table elements</t>
+  </si>
+  <si>
+    <t>POLICY ID</t>
+  </si>
+  <si>
+    <t>TERM</t>
+  </si>
+  <si>
+    <t>TOTAL AMOUNT</t>
+  </si>
+  <si>
+    <t>PER MONTH</t>
+  </si>
+  <si>
+    <t>PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>COVERAGE</t>
+  </si>
+  <si>
+    <t>AGE LIMIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,7 +260,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,6 +328,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -746,7 +776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537CDB81-5D67-4BF2-A179-463C842E8906}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -841,7 +871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47853F6E-6258-4352-84CB-82EF86CB5F5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -918,7 +948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF84665-AAFB-4BC2-ADC5-B1C46716C0FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -964,68 +994,101 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0F5754-5A15-4707-A7D4-FA4309D5767D}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1034,10 +1097,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D539863-51FD-471B-AEFF-0A77A00EDEC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
payment page of client
</commit_message>
<xml_diff>
--- a/src/test/resources/Life Insurance.xlsx
+++ b/src/test/resources/Life Insurance.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A14D67A-FBD7-4DFB-B0D6-CDAFD40D47E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
+    <workbookView xWindow="1560" yWindow="1092" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddClient" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Client Password</t>
   </si>
@@ -231,12 +232,15 @@
   </si>
   <si>
     <t>AGE LIMIT</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -608,7 +612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -776,7 +780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -871,11 +875,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,7 +893,7 @@
     <col min="8" max="8" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -914,8 +918,11 @@
       <c r="H1" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -939,6 +946,9 @@
       </c>
       <c r="H2" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7900</v>
       </c>
     </row>
   </sheetData>
@@ -948,7 +958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -994,10 +1004,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Client Information test commit
</commit_message>
<xml_diff>
--- a/src/test/resources/Life Insurance.xlsx
+++ b/src/test/resources/Life Insurance.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A14D67A-FBD7-4DFB-B0D6-CDAFD40D47E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E36B20-E158-4EA5-AB3C-2C6FC73FE374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1092" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddClient" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="SearchPage" sheetId="3" r:id="rId4"/>
     <sheet name="policy" sheetId="4" r:id="rId5"/>
     <sheet name="Agents" sheetId="5" r:id="rId6"/>
+    <sheet name="Client" sheetId="7" r:id="rId7"/>
+    <sheet name="Nominee" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>Client Password</t>
   </si>
@@ -235,6 +237,48 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Yogi</t>
+  </si>
+  <si>
+    <t>Choose file</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth date </t>
+  </si>
+  <si>
+    <t>Marital status</t>
+  </si>
+  <si>
+    <t>National ID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Rashmi</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Birth date</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>C:\Users\sunit\Downloads\1.png</t>
   </si>
 </sst>
 </file>
@@ -311,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,6 +377,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,29 +661,29 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="13" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.5546875" customWidth="1"/>
+    <col min="13" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.36328125" customWidth="1"/>
+    <col min="17" max="17" width="19.6328125" customWidth="1"/>
+    <col min="18" max="18" width="7.54296875" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -697,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -756,7 +801,7 @@
         <v>8877665544</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -787,20 +832,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -832,7 +877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -864,7 +909,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -878,22 +923,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
+    <col min="8" max="8" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -922,7 +967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -965,15 +1010,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -987,7 +1032,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1011,15 +1056,15 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>61</v>
       </c>
@@ -1048,7 +1093,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1059,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1070,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1081,22 +1126,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1114,12 +1159,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1136,7 +1181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1144,12 +1189,174 @@
         <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F7F7D7-F6EB-4030-9CF4-6842F9C1D3FE}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>777</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="9">
+        <v>35068</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>1234</v>
+      </c>
+      <c r="H2">
+        <v>7894561238</v>
+      </c>
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2">
+        <v>555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6B52EC-CE1D-454F-9894-031D17AAD959}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="9">
+        <v>35547</v>
+      </c>
+      <c r="D2">
+        <v>345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>7894568564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>